<commit_message>
Code correction + adding/modif/rename dataset
</commit_message>
<xml_diff>
--- a/plots/alerts_ech.xlsx
+++ b/plots/alerts_ech.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0D6555B187D0560B539B3811595ED87656CDACCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8074D2DF-8F69-3B4C-8A10-75A17279935F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_0E55D6AD87205348F31B3F11595ED87656CD6549" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33BEB7A4-DDD5-9F41-8A6C-3B73D9BF3891}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>A1-12h</t>
   </si>
@@ -167,6 +167,153 @@
   </si>
   <si>
     <t>A7+12h</t>
+  </si>
+  <si>
+    <t>A8-12h</t>
+  </si>
+  <si>
+    <t>A8-6h</t>
+  </si>
+  <si>
+    <t>A8-3h</t>
+  </si>
+  <si>
+    <t>Dimanche21 Aout 15h - 21h</t>
+  </si>
+  <si>
+    <t>A8+3h</t>
+  </si>
+  <si>
+    <t>A8+6h</t>
+  </si>
+  <si>
+    <t>A8+12h</t>
+  </si>
+  <si>
+    <t>A9-12h</t>
+  </si>
+  <si>
+    <t>A9-6h</t>
+  </si>
+  <si>
+    <t>A9-3h</t>
+  </si>
+  <si>
+    <t>Jeudi1 Septembre 6h - 12h</t>
+  </si>
+  <si>
+    <t>A9+3h</t>
+  </si>
+  <si>
+    <t>A9+6h</t>
+  </si>
+  <si>
+    <t>A9+12h</t>
+  </si>
+  <si>
+    <t>A10-12h</t>
+  </si>
+  <si>
+    <t>A10-6h</t>
+  </si>
+  <si>
+    <t>A10-3h</t>
+  </si>
+  <si>
+    <t>Samedi24 Septembre 10h - 16h</t>
+  </si>
+  <si>
+    <t>A10+3h</t>
+  </si>
+  <si>
+    <t>A10+6h</t>
+  </si>
+  <si>
+    <t>A10+12h</t>
+  </si>
+  <si>
+    <t>A11-12h</t>
+  </si>
+  <si>
+    <t>A11-6h</t>
+  </si>
+  <si>
+    <t>A11-3h</t>
+  </si>
+  <si>
+    <t>Dimanche9 Octobre 12h - 18h</t>
+  </si>
+  <si>
+    <t>A11+3h</t>
+  </si>
+  <si>
+    <t>A11+6h</t>
+  </si>
+  <si>
+    <t>A11+12h</t>
+  </si>
+  <si>
+    <t>A12-12h</t>
+  </si>
+  <si>
+    <t>A12-6h</t>
+  </si>
+  <si>
+    <t>A12-3h</t>
+  </si>
+  <si>
+    <t>Mercredi19 Octobre 17h - 23h</t>
+  </si>
+  <si>
+    <t>A12+3h</t>
+  </si>
+  <si>
+    <t>A12+6h</t>
+  </si>
+  <si>
+    <t>A12+12h</t>
+  </si>
+  <si>
+    <t>A13-12h</t>
+  </si>
+  <si>
+    <t>A13-6h</t>
+  </si>
+  <si>
+    <t>A13-3h</t>
+  </si>
+  <si>
+    <t>Samedi5 Novembre 16h - 22h</t>
+  </si>
+  <si>
+    <t>A13+3h</t>
+  </si>
+  <si>
+    <t>A13+6h</t>
+  </si>
+  <si>
+    <t>A13+12h</t>
+  </si>
+  <si>
+    <t>A14-12h</t>
+  </si>
+  <si>
+    <t>A14-6h</t>
+  </si>
+  <si>
+    <t>A14-3h</t>
+  </si>
+  <si>
+    <t>Mardi15 Novembre 17h - 23h</t>
+  </si>
+  <si>
+    <t>A14+3h</t>
+  </si>
+  <si>
+    <t>A14+6h</t>
+  </si>
+  <si>
+    <t>A14+12h</t>
   </si>
   <si>
     <t>ECHL01</t>
@@ -560,15 +707,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:CU11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:CU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -717,52 +864,199 @@
       <c r="AX1" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="AY1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1">
-        <v>1.829696077286038</v>
+        <v>-8.5820673740887656</v>
       </c>
       <c r="C2" s="1">
-        <v>13.064452633904869</v>
+        <v>-11.914904261040309</v>
       </c>
       <c r="D2" s="1">
-        <v>1.9744918116057919</v>
+        <v>-6.9762427630265478</v>
       </c>
       <c r="E2" s="1">
-        <v>-24.86519857722195</v>
+        <v>-54.249639592541541</v>
       </c>
       <c r="F2" s="1">
-        <v>-14.336284389938591</v>
+        <v>-37.686237215743198</v>
       </c>
       <c r="G2" s="1">
-        <v>-12.391000967443221</v>
+        <v>-39.632728375714073</v>
       </c>
       <c r="H2" s="1">
-        <v>-15.73217206124073</v>
+        <v>-39.150866958353582</v>
       </c>
       <c r="I2" s="1">
-        <v>-7.4819355618781236</v>
+        <v>0.95846278639097893</v>
       </c>
       <c r="J2" s="1">
-        <v>-1.9816609447655369</v>
+        <v>-0.95615134692624382</v>
       </c>
       <c r="K2" s="1">
-        <v>1.6030321949220701</v>
+        <v>0.57138301265015412</v>
       </c>
       <c r="L2" s="1">
-        <v>-14.62470013584208</v>
+        <v>-25.918495297805642</v>
       </c>
       <c r="M2" s="1">
-        <v>15.557063510015331</v>
+        <v>7.3517640539375693</v>
       </c>
       <c r="N2" s="1">
-        <v>19.877004173072692</v>
+        <v>18.426545129275471</v>
       </c>
       <c r="O2" s="1">
-        <v>19.96296765654261</v>
+        <v>12.67620906527868</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -772,25 +1066,25 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1">
-        <v>9.5054404385323181</v>
+        <v>-19.636518305362429</v>
       </c>
       <c r="X2" s="1">
-        <v>8.0879018377085785</v>
+        <v>-25.01712435394483</v>
       </c>
       <c r="Y2" s="1">
-        <v>6.3580453727986459</v>
+        <v>-31.349754633379391</v>
       </c>
       <c r="Z2" s="1">
-        <v>-7.7902621722846428</v>
+        <v>-57.495612935572829</v>
       </c>
       <c r="AA2" s="1">
-        <v>-7.848033759970316</v>
+        <v>-27.241576242147339</v>
       </c>
       <c r="AB2" s="1">
-        <v>-22.82144588348546</v>
+        <v>-17.530022534729149</v>
       </c>
       <c r="AC2" s="1">
-        <v>-18.37224270083669</v>
+        <v>-15.156701882783439</v>
       </c>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
@@ -800,245 +1094,371 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1">
-        <v>-36.665435829621927</v>
+        <v>-4.0593419548188656</v>
       </c>
       <c r="AL2" s="1">
-        <v>-41.876204436579783</v>
+        <v>-2.8338602477019359</v>
       </c>
       <c r="AM2" s="1">
-        <v>-48.825279332880463</v>
+        <v>-5.0955786640925478</v>
       </c>
       <c r="AN2" s="1">
-        <v>-48.967933503888872</v>
+        <v>-15.232292460015231</v>
       </c>
       <c r="AO2" s="1">
-        <v>-47.542823499107669</v>
+        <v>-17.127444369521239</v>
       </c>
       <c r="AP2" s="1">
-        <v>-57.156951531081823</v>
+        <v>-17.373228346456688</v>
       </c>
       <c r="AQ2" s="1">
-        <v>-48.100038174633482</v>
+        <v>-15.86577067748617</v>
       </c>
       <c r="AR2" s="1">
-        <v>-27.790225976567161</v>
+        <v>3.0728681645763261</v>
       </c>
       <c r="AS2" s="1">
-        <v>-32.959907398113927</v>
+        <v>3.4670822290517118</v>
       </c>
       <c r="AT2" s="1">
-        <v>-35.172370027127727</v>
+        <v>3.3838049781850441</v>
       </c>
       <c r="AU2" s="1">
-        <v>-36.989712019039338</v>
+        <v>57.12890625</v>
       </c>
       <c r="AV2" s="1">
-        <v>-40.555394886103549</v>
+        <v>55.663257517936181</v>
       </c>
       <c r="AW2" s="1">
-        <v>-43.697694111140379</v>
+        <v>55.007381889763771</v>
       </c>
       <c r="AX2" s="1">
-        <v>-36.827725787593643</v>
+        <v>54.196363304093552</v>
+      </c>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+      <c r="BR2" s="1"/>
+      <c r="BS2" s="1"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="1"/>
+      <c r="CJ2" s="1"/>
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1">
+        <v>12.3224799651093</v>
+      </c>
+      <c r="CP2" s="1">
+        <v>15.97501435956347</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>21.090668619069</v>
+      </c>
+      <c r="CR2" s="1">
+        <v>54.920767306088408</v>
+      </c>
+      <c r="CS2" s="1">
+        <v>129.02119793685341</v>
+      </c>
+      <c r="CT2" s="1">
+        <v>108.28469642992491</v>
+      </c>
+      <c r="CU2" s="1">
+        <v>82.36492590385761</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1">
-        <v>-19.768852363252979</v>
+        <v>-17.789749933523709</v>
       </c>
       <c r="C3" s="1">
-        <v>-31.651613474822408</v>
+        <v>-27.858034599607642</v>
       </c>
       <c r="D3" s="1">
-        <v>-50.271766524793982</v>
+        <v>-46.54247247602752</v>
       </c>
       <c r="E3" s="1">
-        <v>-89.495806747039168</v>
+        <v>-116.167630224063</v>
       </c>
       <c r="F3" s="1">
-        <v>-67.806197144045569</v>
+        <v>-76.1920742791621</v>
       </c>
       <c r="G3" s="1">
-        <v>-33.357309736875592</v>
+        <v>-34.320647332939537</v>
       </c>
       <c r="H3" s="1">
-        <v>-15.33903542965056</v>
+        <v>-13.21844206970783</v>
       </c>
       <c r="I3" s="1">
-        <v>-5.7983579669700758</v>
+        <v>4.4413532713994748</v>
       </c>
       <c r="J3" s="1">
-        <v>-1.9609375844040171</v>
+        <v>11.91408230736466</v>
       </c>
       <c r="K3" s="1">
-        <v>-5.875693139844083</v>
+        <v>5.6302023256539044</v>
       </c>
       <c r="L3" s="1">
-        <v>-27.602818833909382</v>
+        <v>5.0989964740981746</v>
       </c>
       <c r="M3" s="1">
-        <v>-0.1946063514170967</v>
+        <v>36.807627670885203</v>
       </c>
       <c r="N3" s="1">
-        <v>-0.16840768111877161</v>
+        <v>25.576009044906211</v>
       </c>
       <c r="O3" s="1">
-        <v>-3.341900749034711</v>
+        <v>9.6347873819368619</v>
       </c>
       <c r="P3" s="1">
-        <v>-20.904736389087649</v>
+        <v>-11.409626157539741</v>
       </c>
       <c r="Q3" s="1">
-        <v>-24.94325887124181</v>
+        <v>-12.280218032195799</v>
       </c>
       <c r="R3" s="1">
-        <v>-23.861895684866312</v>
+        <v>-11.473709030888941</v>
       </c>
       <c r="S3" s="1">
-        <v>-36.054424972122597</v>
+        <v>-20.273424474824939</v>
       </c>
       <c r="T3" s="1">
-        <v>-44.329061732125673</v>
+        <v>-40.452428476380561</v>
       </c>
       <c r="U3" s="1">
-        <v>-34.876427741405202</v>
+        <v>-32.10772768834336</v>
       </c>
       <c r="V3" s="1">
-        <v>-33.699629414315993</v>
+        <v>-27.738649671814141</v>
       </c>
       <c r="W3" s="1">
-        <v>10.060532289743501</v>
+        <v>0.40725321126259628</v>
       </c>
       <c r="X3" s="1">
-        <v>6.125086075517312</v>
+        <v>-6.6252639423673996</v>
       </c>
       <c r="Y3" s="1">
-        <v>-2.3067998176770468</v>
+        <v>-9.9449513611341622</v>
       </c>
       <c r="Z3" s="1">
-        <v>2.7252934674898852</v>
+        <v>-11.04595800130306</v>
       </c>
       <c r="AA3" s="1">
-        <v>-10.3237336510505</v>
+        <v>-18.564410880563081</v>
       </c>
       <c r="AB3" s="1">
-        <v>-6.5135523713396868</v>
+        <v>-12.07603428997392</v>
       </c>
       <c r="AC3" s="1">
-        <v>-15.472951063098369</v>
+        <v>-12.474012474012479</v>
       </c>
       <c r="AD3" s="1">
-        <v>-17.197799661064121</v>
+        <v>-10.32705967334163</v>
       </c>
       <c r="AE3" s="1">
-        <v>-18.623173250551218</v>
+        <v>-12.168741237945531</v>
       </c>
       <c r="AF3" s="1">
-        <v>-19.171818556501069</v>
+        <v>-11.27558332855587</v>
       </c>
       <c r="AG3" s="1">
-        <v>-21.15175752615152</v>
+        <v>-18.665026986404321</v>
       </c>
       <c r="AH3" s="1">
-        <v>-21.3749255030522</v>
+        <v>-18.504220853296822</v>
       </c>
       <c r="AI3" s="1">
-        <v>-24.50248604898675</v>
+        <v>-20.940882898086649</v>
       </c>
       <c r="AJ3" s="1">
-        <v>-20.221883338721469</v>
+        <v>-17.409717409717398</v>
       </c>
       <c r="AK3" s="1">
-        <v>-7.3114379332947248</v>
+        <v>-6.920633781334673</v>
       </c>
       <c r="AL3" s="1">
-        <v>-26.596159571123021</v>
+        <v>-23.736751684947791</v>
       </c>
       <c r="AM3" s="1">
-        <v>-25.267818576528992</v>
+        <v>-13.156621123562029</v>
       </c>
       <c r="AN3" s="1">
-        <v>-22.588258230409309</v>
+        <v>-12.17924488681702</v>
       </c>
       <c r="AO3" s="1">
-        <v>-24.85332857729761</v>
+        <v>-15.838796090585779</v>
       </c>
       <c r="AP3" s="1">
-        <v>-21.882050809215951</v>
+        <v>-13.294834236095021</v>
       </c>
       <c r="AQ3" s="1">
-        <v>-14.758103332531119</v>
+        <v>-5.9720501684054401</v>
       </c>
       <c r="AR3" s="1">
-        <v>-13.023447854500059</v>
+        <v>2.5773013096307529</v>
       </c>
       <c r="AS3" s="1">
-        <v>-18.615610550464218</v>
+        <v>2.0242014709396532</v>
       </c>
       <c r="AT3" s="1">
-        <v>-19.545033688197211</v>
+        <v>1.7440893618370941</v>
       </c>
       <c r="AU3" s="1">
-        <v>-23.001217114325492</v>
+        <v>29.814278187565861</v>
       </c>
       <c r="AV3" s="1">
-        <v>-23.906912840560619</v>
+        <v>30.418401744993051</v>
       </c>
       <c r="AW3" s="1">
-        <v>-19.821293901079471</v>
+        <v>30.650877587758782</v>
       </c>
       <c r="AX3" s="1">
-        <v>-16.247767766522379</v>
+        <v>30.134906563958349</v>
+      </c>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BO3" s="1"/>
+      <c r="BP3" s="1"/>
+      <c r="BQ3" s="1"/>
+      <c r="BR3" s="1"/>
+      <c r="BS3" s="1"/>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+      <c r="BV3" s="1"/>
+      <c r="BW3" s="1"/>
+      <c r="BX3" s="1"/>
+      <c r="BY3" s="1"/>
+      <c r="BZ3" s="1"/>
+      <c r="CA3" s="1"/>
+      <c r="CB3" s="1"/>
+      <c r="CC3" s="1"/>
+      <c r="CD3" s="1"/>
+      <c r="CE3" s="1"/>
+      <c r="CF3" s="1"/>
+      <c r="CG3" s="1"/>
+      <c r="CH3" s="1"/>
+      <c r="CI3" s="1"/>
+      <c r="CJ3" s="1"/>
+      <c r="CK3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CM3" s="1"/>
+      <c r="CN3" s="1"/>
+      <c r="CO3" s="1">
+        <v>-25.438294224433541</v>
+      </c>
+      <c r="CP3" s="1">
+        <v>-26.200615827766882</v>
+      </c>
+      <c r="CQ3" s="1">
+        <v>-25.462733841433241</v>
+      </c>
+      <c r="CR3" s="1">
+        <v>-45.060966758600657</v>
+      </c>
+      <c r="CS3" s="1">
+        <v>-45.152361238145659</v>
+      </c>
+      <c r="CT3" s="1">
+        <v>-47.157867853624722</v>
+      </c>
+      <c r="CU3" s="1">
+        <v>-45.200777520791299</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1">
-        <v>-14.93110342954804</v>
+        <v>-9.2726242206687992</v>
       </c>
       <c r="C4" s="1">
-        <v>-25.440058796241171</v>
+        <v>-20.538644894380681</v>
       </c>
       <c r="D4" s="1">
-        <v>-33.23498722732959</v>
+        <v>-28.0565897244974</v>
       </c>
       <c r="E4" s="1">
-        <v>-47.801123322584253</v>
+        <v>-23.21029764080075</v>
       </c>
       <c r="F4" s="1">
-        <v>-19.1697487440955</v>
+        <v>11.27734398283363</v>
       </c>
       <c r="G4" s="1">
-        <v>-23.230368478656569</v>
+        <v>-13.38715836561015</v>
       </c>
       <c r="H4" s="1">
-        <v>-9.5872178729160531</v>
+        <v>-13.414199650191099</v>
       </c>
       <c r="I4" s="1">
-        <v>-7.7455718391042634</v>
+        <v>-8.0423917570577519</v>
       </c>
       <c r="J4" s="1">
-        <v>-7.2364142188973339</v>
+        <v>-19.16938068651778</v>
       </c>
       <c r="K4" s="1">
-        <v>-5.6022341235779791</v>
+        <v>-24.118384060628291</v>
       </c>
       <c r="L4" s="1">
-        <v>-7.9071733897742389</v>
+        <v>9.3461725198252257</v>
       </c>
       <c r="M4" s="1">
-        <v>6.201269783812883</v>
+        <v>33.260350318471339</v>
       </c>
       <c r="N4" s="1">
-        <v>5.7897645162810791</v>
+        <v>40.860820595333863</v>
       </c>
       <c r="O4" s="1">
-        <v>-1.942613006374589</v>
+        <v>17.78976991588322</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1048,287 +1468,413 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1">
-        <v>-13.81900460344144</v>
+        <v>-10.70866141732283</v>
       </c>
       <c r="X4" s="1">
-        <v>-29.701479467502761</v>
+        <v>-20.781742825117949</v>
       </c>
       <c r="Y4" s="1">
-        <v>-43.25506881879727</v>
+        <v>-30.055380355357279</v>
       </c>
       <c r="Z4" s="1">
-        <v>-87.497716894977174</v>
+        <v>-102.14398830551831</v>
       </c>
       <c r="AA4" s="1">
-        <v>-48.865965380151607</v>
+        <v>-49.25691699604743</v>
       </c>
       <c r="AB4" s="1">
-        <v>-42.050232618760241</v>
+        <v>-45.607164027436689</v>
       </c>
       <c r="AC4" s="1">
-        <v>-37.990882839344323</v>
+        <v>-42.5647476690839</v>
       </c>
       <c r="AD4" s="1">
-        <v>-59.787969490751067</v>
+        <v>-44.513928930330628</v>
       </c>
       <c r="AE4" s="1">
-        <v>-66.410012753940833</v>
+        <v>-50.197070388851841</v>
       </c>
       <c r="AF4" s="1">
-        <v>-68.494082802192864</v>
+        <v>-48.778912082888908</v>
       </c>
       <c r="AG4" s="1">
-        <v>-75.024304225032282</v>
+        <v>-68.295585555431586</v>
       </c>
       <c r="AH4" s="1">
-        <v>-72.758496447901251</v>
+        <v>-65.440036664105577</v>
       </c>
       <c r="AI4" s="1">
-        <v>-67.299667463272755</v>
+        <v>-58.161176882978843</v>
       </c>
       <c r="AJ4" s="1">
-        <v>-62.259798386478707</v>
+        <v>-54.94955109350996</v>
       </c>
       <c r="AK4" s="1">
-        <v>-34.007314771118459</v>
+        <v>14.823694029850749</v>
       </c>
       <c r="AL4" s="1">
-        <v>-33.977066106198251</v>
+        <v>20.981956234270349</v>
       </c>
       <c r="AM4" s="1">
-        <v>-42.469150775722987</v>
+        <v>19.413149223285739</v>
       </c>
       <c r="AN4" s="1">
-        <v>-78.549247725682307</v>
+        <v>34.549299497753111</v>
       </c>
       <c r="AO4" s="1">
-        <v>-32.396750781310537</v>
+        <v>36.75578337784053</v>
       </c>
       <c r="AP4" s="1">
-        <v>-39.339255968906159</v>
+        <v>5.1719797697782379</v>
       </c>
       <c r="AQ4" s="1">
-        <v>-35.115614540693016</v>
+        <v>4.1918934033603152</v>
       </c>
       <c r="AR4" s="1">
-        <v>-31.4884789959189</v>
+        <v>-7.6844008195517732</v>
       </c>
       <c r="AS4" s="1">
-        <v>-41.758155170048028</v>
+        <v>-14.619062961502109</v>
       </c>
       <c r="AT4" s="1">
-        <v>-46.688602028565533</v>
+        <v>-14.175552873005209</v>
       </c>
       <c r="AU4" s="1">
-        <v>-60.530883227300379</v>
+        <v>-63.033919597989943</v>
       </c>
       <c r="AV4" s="1">
-        <v>-58.821809679657257</v>
+        <v>-69.220110847189218</v>
       </c>
       <c r="AW4" s="1">
-        <v>-53.146323787007589</v>
+        <v>-66.993327773144287</v>
       </c>
       <c r="AX4" s="1">
-        <v>-42.715812358308114</v>
+        <v>-70.86499123319696</v>
+      </c>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1"/>
+      <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
+      <c r="BL4" s="1"/>
+      <c r="BM4" s="1"/>
+      <c r="BN4" s="1"/>
+      <c r="BO4" s="1"/>
+      <c r="BP4" s="1"/>
+      <c r="BQ4" s="1"/>
+      <c r="BR4" s="1"/>
+      <c r="BS4" s="1"/>
+      <c r="BT4" s="1"/>
+      <c r="BU4" s="1"/>
+      <c r="BV4" s="1"/>
+      <c r="BW4" s="1"/>
+      <c r="BX4" s="1"/>
+      <c r="BY4" s="1"/>
+      <c r="BZ4" s="1"/>
+      <c r="CA4" s="1"/>
+      <c r="CB4" s="1"/>
+      <c r="CC4" s="1"/>
+      <c r="CD4" s="1"/>
+      <c r="CE4" s="1"/>
+      <c r="CF4" s="1"/>
+      <c r="CG4" s="1"/>
+      <c r="CH4" s="1"/>
+      <c r="CI4" s="1"/>
+      <c r="CJ4" s="1"/>
+      <c r="CK4" s="1"/>
+      <c r="CL4" s="1"/>
+      <c r="CM4" s="1"/>
+      <c r="CN4" s="1"/>
+      <c r="CO4" s="1">
+        <v>-8.1388479354224899</v>
+      </c>
+      <c r="CP4" s="1">
+        <v>-18.830667441168551</v>
+      </c>
+      <c r="CQ4" s="1">
+        <v>-31.708054460916159</v>
+      </c>
+      <c r="CR4" s="1">
+        <v>-49.660268387973488</v>
+      </c>
+      <c r="CS4" s="1">
+        <v>44.029311590463408</v>
+      </c>
+      <c r="CT4" s="1">
+        <v>51.546826389090803</v>
+      </c>
+      <c r="CU4" s="1">
+        <v>32.197631527858682</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1">
-        <v>-43.19137803027553</v>
+        <v>-55.646703573225963</v>
       </c>
       <c r="C5" s="1">
-        <v>-38.753806735842993</v>
+        <v>-58.89736344515498</v>
       </c>
       <c r="D5" s="1">
-        <v>-47.245255233612298</v>
+        <v>-67.916157105884352</v>
       </c>
       <c r="E5" s="1">
-        <v>-68.635445579883807</v>
+        <v>-101.06446764937201</v>
       </c>
       <c r="F5" s="1">
-        <v>-26.121249764111312</v>
+        <v>-36.885364559038777</v>
       </c>
       <c r="G5" s="1">
-        <v>-7.8157284812182901</v>
+        <v>-49.918794833945611</v>
       </c>
       <c r="H5" s="1">
-        <v>-8.609746023304476</v>
+        <v>-48.685088655453541</v>
       </c>
       <c r="I5" s="1">
-        <v>61.0683039401709</v>
+        <v>25.191298615688869</v>
       </c>
       <c r="J5" s="1">
-        <v>77.325632153803028</v>
+        <v>32.086687438190552</v>
       </c>
       <c r="K5" s="1">
-        <v>86.394358897340524</v>
+        <v>37.529663630755827</v>
       </c>
       <c r="L5" s="1">
-        <v>255.65609100747619</v>
+        <v>197.74752059169609</v>
       </c>
       <c r="M5" s="1">
-        <v>161.22628638445079</v>
+        <v>189.55010769342459</v>
       </c>
       <c r="N5" s="1">
-        <v>71.328306928283112</v>
+        <v>94.052199614704563</v>
       </c>
       <c r="O5" s="1">
-        <v>29.79373194237737</v>
+        <v>34.261846859843651</v>
       </c>
       <c r="P5" s="1">
-        <v>2.1877617281900821</v>
+        <v>-3.3905838280580198</v>
       </c>
       <c r="Q5" s="1">
-        <v>-6.1418615867362654</v>
+        <v>-2.6028933711005129</v>
       </c>
       <c r="R5" s="1">
-        <v>-9.8190685677312075</v>
+        <v>-2.327635874783931</v>
       </c>
       <c r="S5" s="1">
-        <v>-16.283753635642519</v>
+        <v>9.5136670216542409</v>
       </c>
       <c r="T5" s="1">
-        <v>15.026247479546671</v>
+        <v>40.064031523211419</v>
       </c>
       <c r="U5" s="1">
-        <v>11.99311835048683</v>
+        <v>-12.75218880852684</v>
       </c>
       <c r="V5" s="1">
-        <v>-0.1252566581558705</v>
+        <v>-24.489722629965311</v>
       </c>
       <c r="W5" s="1">
-        <v>5.962449978488543</v>
+        <v>-11.900659254855681</v>
       </c>
       <c r="X5" s="1">
-        <v>-53.561746333345752</v>
+        <v>-52.593436733432483</v>
       </c>
       <c r="Y5" s="1">
-        <v>-53.755423261017462</v>
+        <v>-31.061032863849771</v>
       </c>
       <c r="Z5" s="1">
-        <v>-73.172511119623735</v>
+        <v>-65.024815938654058</v>
       </c>
       <c r="AA5" s="1">
-        <v>-44.418148785618669</v>
+        <v>-15.837979875664921</v>
       </c>
       <c r="AB5" s="1">
-        <v>-2.728730504542316</v>
+        <v>-6.0411463907717948</v>
       </c>
       <c r="AC5" s="1">
-        <v>3.7729670827331132</v>
+        <v>-1.7721871442727419</v>
       </c>
       <c r="AD5" s="1">
-        <v>-35.939838620412857</v>
+        <v>-26.272189349112431</v>
       </c>
       <c r="AE5" s="1">
-        <v>-47.179945500267237</v>
+        <v>-43.458454810495631</v>
       </c>
       <c r="AF5" s="1">
-        <v>-54.114095407928531</v>
+        <v>-53.411008874612079</v>
       </c>
       <c r="AG5" s="1">
-        <v>-66.022811104317299</v>
+        <v>-85.201564141267028</v>
       </c>
       <c r="AH5" s="1">
-        <v>-64.239792780622423</v>
+        <v>-82.905688931691543</v>
       </c>
       <c r="AI5" s="1">
-        <v>-62.929560360558632</v>
+        <v>-76.398535426164472</v>
       </c>
       <c r="AJ5" s="1">
-        <v>-58.075753836255103</v>
+        <v>-64.648779400999373</v>
       </c>
       <c r="AK5" s="1">
-        <v>-19.414430462880979</v>
+        <v>38.41899203472736</v>
       </c>
       <c r="AL5" s="1">
-        <v>-34.418585137810553</v>
+        <v>41.549197909428713</v>
       </c>
       <c r="AM5" s="1">
-        <v>-46.972659066948673</v>
+        <v>31.78776163178242</v>
       </c>
       <c r="AN5" s="1">
-        <v>-55.072244248380613</v>
+        <v>81.136896636214075</v>
       </c>
       <c r="AO5" s="1">
-        <v>-51.168085069454477</v>
+        <v>56.137983763970389</v>
       </c>
       <c r="AP5" s="1">
-        <v>-30.340446310990121</v>
+        <v>50.664536277144308</v>
       </c>
       <c r="AQ5" s="1">
-        <v>-27.459965312492841</v>
+        <v>41.833851978259943</v>
       </c>
       <c r="AR5" s="1">
-        <v>46.310707399282379</v>
+        <v>21.112443000373759</v>
       </c>
       <c r="AS5" s="1">
-        <v>63.187532088801731</v>
+        <v>18.84887987746977</v>
       </c>
       <c r="AT5" s="1">
-        <v>28.434619739604759</v>
+        <v>13.682740171903159</v>
       </c>
       <c r="AU5" s="1">
-        <v>29.795677423325252</v>
+        <v>79.523522316043426</v>
       </c>
       <c r="AV5" s="1">
-        <v>22.31763315079203</v>
+        <v>74.742343934040051</v>
       </c>
       <c r="AW5" s="1">
-        <v>31.758053520676441</v>
+        <v>78.136580746108862</v>
       </c>
       <c r="AX5" s="1">
-        <v>31.517757623050141</v>
+        <v>70.337022017549884</v>
+      </c>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="1"/>
+      <c r="BV5" s="1"/>
+      <c r="BW5" s="1"/>
+      <c r="BX5" s="1"/>
+      <c r="BY5" s="1"/>
+      <c r="BZ5" s="1"/>
+      <c r="CA5" s="1"/>
+      <c r="CB5" s="1"/>
+      <c r="CC5" s="1"/>
+      <c r="CD5" s="1"/>
+      <c r="CE5" s="1"/>
+      <c r="CF5" s="1"/>
+      <c r="CG5" s="1"/>
+      <c r="CH5" s="1"/>
+      <c r="CI5" s="1"/>
+      <c r="CJ5" s="1"/>
+      <c r="CK5" s="1"/>
+      <c r="CL5" s="1"/>
+      <c r="CM5" s="1"/>
+      <c r="CN5" s="1"/>
+      <c r="CO5" s="1">
+        <v>6.6441756794599183</v>
+      </c>
+      <c r="CP5" s="1">
+        <v>-3.6247361543873802</v>
+      </c>
+      <c r="CQ5" s="1">
+        <v>-0.41388876459796597</v>
+      </c>
+      <c r="CR5" s="1">
+        <v>-3.811490799849794</v>
+      </c>
+      <c r="CS5" s="1">
+        <v>20.112839280268389</v>
+      </c>
+      <c r="CT5" s="1">
+        <v>8.5118801873496253</v>
+      </c>
+      <c r="CU5" s="1">
+        <v>17.626315850424429</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1">
-        <v>-14.212884386250151</v>
+        <v>-15.26533477816273</v>
       </c>
       <c r="C6" s="1">
-        <v>-21.917251447302981</v>
+        <v>-26.528149798483</v>
       </c>
       <c r="D6" s="1">
-        <v>-24.356608438295371</v>
+        <v>-22.309084328628291</v>
       </c>
       <c r="E6" s="1">
-        <v>-31.816193439685339</v>
+        <v>-49.404761904761898</v>
       </c>
       <c r="F6" s="1">
-        <v>-29.89125884794797</v>
+        <v>-36.807101326102497</v>
       </c>
       <c r="G6" s="1">
-        <v>-18.272108825358568</v>
+        <v>-21.841047138335181</v>
       </c>
       <c r="H6" s="1">
-        <v>-12.988897980014389</v>
+        <v>-12.157564124934559</v>
       </c>
       <c r="I6" s="1">
-        <v>-15.58026065337687</v>
+        <v>-3.8908589440504389</v>
       </c>
       <c r="J6" s="1">
-        <v>-8.5965725471068879</v>
+        <v>1.812743946942533</v>
       </c>
       <c r="K6" s="1">
-        <v>-9.5808268536421526</v>
+        <v>6.509519297036527</v>
       </c>
       <c r="L6" s="1">
-        <v>8.8547815820545606E-2</v>
+        <v>39.457678661936143</v>
       </c>
       <c r="M6" s="1">
-        <v>-12.49692952981253</v>
+        <v>16.89320388349514</v>
       </c>
       <c r="N6" s="1">
-        <v>-0.71709191382808357</v>
+        <v>-2.765416401780044</v>
       </c>
       <c r="O6" s="1">
-        <v>18.127907738680289</v>
+        <v>-6.9573283858998147</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1338,25 +1884,25 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1">
-        <v>-6.3562286833794186</v>
+        <v>-6.1000929349652973</v>
       </c>
       <c r="X6" s="1">
-        <v>-13.07155493090133</v>
+        <v>-12.188497876683019</v>
       </c>
       <c r="Y6" s="1">
-        <v>-20.371845000850911</v>
+        <v>-15.633195060315661</v>
       </c>
       <c r="Z6" s="1">
-        <v>-26.86255386048677</v>
+        <v>-12.862196765498661</v>
       </c>
       <c r="AA6" s="1">
-        <v>17.997188632140929</v>
+        <v>43.700261030113957</v>
       </c>
       <c r="AB6" s="1">
-        <v>2.3529517703418259</v>
+        <v>31.481394142338338</v>
       </c>
       <c r="AC6" s="1">
-        <v>3.9403011084625201</v>
+        <v>20.643069440691711</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
@@ -1366,245 +1912,371 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1">
-        <v>-14.158780661432329</v>
+        <v>-12.37677840512761</v>
       </c>
       <c r="AL6" s="1">
-        <v>-12.628221598107579</v>
+        <v>-11.686634837702311</v>
       </c>
       <c r="AM6" s="1">
-        <v>-7.4495633252267188</v>
+        <v>-10.82408895509127</v>
       </c>
       <c r="AN6" s="1">
-        <v>-5.9458514402305633</v>
+        <v>-28.141459744168561</v>
       </c>
       <c r="AO6" s="1">
-        <v>-14.45092077485827</v>
+        <v>-36.149312377210222</v>
       </c>
       <c r="AP6" s="1">
-        <v>-19.805733238569061</v>
+        <v>-48.988631330281997</v>
       </c>
       <c r="AQ6" s="1">
-        <v>-19.24896111263412</v>
+        <v>-60.891520634825213</v>
       </c>
       <c r="AR6" s="1">
-        <v>32.482572309137367</v>
+        <v>8.9191636547089814</v>
       </c>
       <c r="AS6" s="1">
-        <v>32.592492726680447</v>
+        <v>8.6338771106428496</v>
       </c>
       <c r="AT6" s="1">
-        <v>23.74681615236338</v>
+        <v>3.801314316059242</v>
       </c>
       <c r="AU6" s="1">
-        <v>7.4044850114305696</v>
+        <v>14.55261394101877</v>
       </c>
       <c r="AV6" s="1">
-        <v>21.06302762405069</v>
+        <v>44.223962713765083</v>
       </c>
       <c r="AW6" s="1">
-        <v>12.03755891396588</v>
+        <v>39.104889251373628</v>
       </c>
       <c r="AX6" s="1">
-        <v>7.1923024651890284</v>
+        <v>30.37058246073299</v>
+      </c>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="1"/>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+      <c r="BV6" s="1"/>
+      <c r="BW6" s="1"/>
+      <c r="BX6" s="1"/>
+      <c r="BY6" s="1"/>
+      <c r="BZ6" s="1"/>
+      <c r="CA6" s="1"/>
+      <c r="CB6" s="1"/>
+      <c r="CC6" s="1"/>
+      <c r="CD6" s="1"/>
+      <c r="CE6" s="1"/>
+      <c r="CF6" s="1"/>
+      <c r="CG6" s="1"/>
+      <c r="CH6" s="1"/>
+      <c r="CI6" s="1"/>
+      <c r="CJ6" s="1"/>
+      <c r="CK6" s="1"/>
+      <c r="CL6" s="1"/>
+      <c r="CM6" s="1"/>
+      <c r="CN6" s="1"/>
+      <c r="CO6" s="1">
+        <v>-52.721644540361432</v>
+      </c>
+      <c r="CP6" s="1">
+        <v>-55.968798211643197</v>
+      </c>
+      <c r="CQ6" s="1">
+        <v>-59.23713049456105</v>
+      </c>
+      <c r="CR6" s="1">
+        <v>-94.442501398992718</v>
+      </c>
+      <c r="CS6" s="1">
+        <v>-92.10512885940291</v>
+      </c>
+      <c r="CT6" s="1">
+        <v>-86.840180421796902</v>
+      </c>
+      <c r="CU6" s="1">
+        <v>-86.744409384003291</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1">
-        <v>72.164585172650575</v>
+        <v>10.467373477563379</v>
       </c>
       <c r="C7" s="1">
-        <v>76.784882834986973</v>
+        <v>16.902888795953629</v>
       </c>
       <c r="D7" s="1">
-        <v>86.590443363347404</v>
+        <v>19.715359977718968</v>
       </c>
       <c r="E7" s="1">
-        <v>207.95223475937959</v>
+        <v>60.364570522806147</v>
       </c>
       <c r="F7" s="1">
-        <v>143.55963854352709</v>
+        <v>33.434050027490308</v>
       </c>
       <c r="G7" s="1">
-        <v>145.73281567293591</v>
+        <v>40.384311494579798</v>
       </c>
       <c r="H7" s="1">
-        <v>101.09959430043131</v>
+        <v>32.630568469610729</v>
       </c>
       <c r="I7" s="1">
-        <v>-13.967465224357451</v>
+        <v>-15.51291969673526</v>
       </c>
       <c r="J7" s="1">
-        <v>-18.96357816420106</v>
+        <v>-21.16514062670996</v>
       </c>
       <c r="K7" s="1">
-        <v>-15.15511403940811</v>
+        <v>-2.1404380221268959</v>
       </c>
       <c r="L7" s="1">
-        <v>0.58488164502139861</v>
+        <v>40.882953069931382</v>
       </c>
       <c r="M7" s="1">
-        <v>2.718978325271693</v>
+        <v>24.471685131359099</v>
       </c>
       <c r="N7" s="1">
-        <v>-16.16273252036769</v>
+        <v>4.5674808783617067</v>
       </c>
       <c r="O7" s="1">
-        <v>17.248205422459911</v>
+        <v>63.930195403711451</v>
       </c>
       <c r="P7" s="1">
-        <v>-61.926679249351423</v>
+        <v>-63.393163955401199</v>
       </c>
       <c r="Q7" s="1">
-        <v>-58.924921557634249</v>
+        <v>-62.975186001080687</v>
       </c>
       <c r="R7" s="1">
-        <v>-67.728585616531987</v>
+        <v>-73.009053245358288</v>
       </c>
       <c r="S7" s="1">
-        <v>-82.680022074931642</v>
+        <v>-102.512321192451</v>
       </c>
       <c r="T7" s="1">
-        <v>-79.269951923076917</v>
+        <v>-90.065219042658256</v>
       </c>
       <c r="U7" s="1">
-        <v>-77.05426220217862</v>
+        <v>-93.517370140694808</v>
       </c>
       <c r="V7" s="1">
-        <v>-78.71369577348959</v>
+        <v>-96.705957451491841</v>
       </c>
       <c r="W7" s="1">
-        <v>-16.526325346845709</v>
+        <v>-17.477768159282292</v>
       </c>
       <c r="X7" s="1">
-        <v>-9.2102044221708113</v>
+        <v>-21.914686515888921</v>
       </c>
       <c r="Y7" s="1">
-        <v>-19.109594449880191</v>
+        <v>-31.92839707078927</v>
       </c>
       <c r="Z7" s="1">
-        <v>-46.210644285966538</v>
+        <v>-74.059183209486548</v>
       </c>
       <c r="AA7" s="1">
-        <v>-52.53822939552547</v>
+        <v>-80.844243903641797</v>
       </c>
       <c r="AB7" s="1">
-        <v>-49.173710257423771</v>
+        <v>-74.102625873283543</v>
       </c>
       <c r="AC7" s="1">
-        <v>-38.545822884002483</v>
+        <v>-62.527631281221183</v>
       </c>
       <c r="AD7" s="1">
-        <v>-31.852420024488769</v>
+        <v>-23.728191338026232</v>
       </c>
       <c r="AE7" s="1">
-        <v>-56.87295975007325</v>
+        <v>-54.344130610899803</v>
       </c>
       <c r="AF7" s="1">
-        <v>-61.055966175612973</v>
+        <v>-61.503038687682199</v>
       </c>
       <c r="AG7" s="1">
-        <v>-70.584637558850176</v>
+        <v>-92.135929104737983</v>
       </c>
       <c r="AH7" s="1">
-        <v>-65.048454475502453</v>
+        <v>-88.937119833491934</v>
       </c>
       <c r="AI7" s="1">
-        <v>-56.83421415218104</v>
+        <v>-74.771901194273426</v>
       </c>
       <c r="AJ7" s="1">
-        <v>-27.578181542204799</v>
+        <v>-34.243551223801838</v>
       </c>
       <c r="AK7" s="1">
-        <v>39.3921138991672</v>
+        <v>36.025945072456182</v>
       </c>
       <c r="AL7" s="1">
-        <v>53.349576658341981</v>
+        <v>39.961659146192588</v>
       </c>
       <c r="AM7" s="1">
-        <v>74.047952041052426</v>
+        <v>42.219902050481672</v>
       </c>
       <c r="AN7" s="1">
-        <v>131.36503880259551</v>
+        <v>96.737145565734977</v>
       </c>
       <c r="AO7" s="1">
-        <v>90.340834579639505</v>
+        <v>45.884886309719327</v>
       </c>
       <c r="AP7" s="1">
-        <v>58.145865353244318</v>
+        <v>39.992381141669362</v>
       </c>
       <c r="AQ7" s="1">
-        <v>42.504373966010597</v>
+        <v>34.81742723807487</v>
       </c>
       <c r="AR7" s="1">
-        <v>-1.1194569749532739</v>
+        <v>-6.4177662443084246E-2</v>
       </c>
       <c r="AS7" s="1">
-        <v>5.9411887369343379</v>
+        <v>-3.078517191882141</v>
       </c>
       <c r="AT7" s="1">
-        <v>-7.437282882941906</v>
+        <v>10.688925937741461</v>
       </c>
       <c r="AU7" s="1">
-        <v>15.95016559502036</v>
+        <v>63.672275805458654</v>
       </c>
       <c r="AV7" s="1">
-        <v>10.021903948597609</v>
+        <v>53.191991558369438</v>
       </c>
       <c r="AW7" s="1">
-        <v>5.485985412376853</v>
+        <v>44.630090005080937</v>
       </c>
       <c r="AX7" s="1">
-        <v>12.066000663506379</v>
+        <v>42.359953879041903</v>
+      </c>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
+      <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
+      <c r="BV7" s="1"/>
+      <c r="BW7" s="1"/>
+      <c r="BX7" s="1"/>
+      <c r="BY7" s="1"/>
+      <c r="BZ7" s="1"/>
+      <c r="CA7" s="1"/>
+      <c r="CB7" s="1"/>
+      <c r="CC7" s="1"/>
+      <c r="CD7" s="1"/>
+      <c r="CE7" s="1"/>
+      <c r="CF7" s="1"/>
+      <c r="CG7" s="1"/>
+      <c r="CH7" s="1"/>
+      <c r="CI7" s="1"/>
+      <c r="CJ7" s="1"/>
+      <c r="CK7" s="1"/>
+      <c r="CL7" s="1"/>
+      <c r="CM7" s="1"/>
+      <c r="CN7" s="1"/>
+      <c r="CO7" s="1">
+        <v>3.1201128453589351</v>
+      </c>
+      <c r="CP7" s="1">
+        <v>-16.930144412992369</v>
+      </c>
+      <c r="CQ7" s="1">
+        <v>-19.491201224177502</v>
+      </c>
+      <c r="CR7" s="1">
+        <v>-48.012684989429182</v>
+      </c>
+      <c r="CS7" s="1">
+        <v>-48.491167236774281</v>
+      </c>
+      <c r="CT7" s="1">
+        <v>-47.278253126330867</v>
+      </c>
+      <c r="CU7" s="1">
+        <v>-64.498176933410093</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1">
-        <v>-8.6886974952835363</v>
+        <v>-23.241633082179771</v>
       </c>
       <c r="C8" s="1">
-        <v>-13.9716076586566</v>
+        <v>-27.67567253331784</v>
       </c>
       <c r="D8" s="1">
-        <v>-24.927130551664849</v>
+        <v>-40.091653027823227</v>
       </c>
       <c r="E8" s="1">
-        <v>-55.862798885803691</v>
+        <v>-78.012366999052972</v>
       </c>
       <c r="F8" s="1">
-        <v>-30.087333370031001</v>
+        <v>-49.303322615219727</v>
       </c>
       <c r="G8" s="1">
-        <v>-17.84813804484466</v>
+        <v>-38.524657421842939</v>
       </c>
       <c r="H8" s="1">
-        <v>-12.52347020451667</v>
+        <v>-44.763903462749219</v>
       </c>
       <c r="I8" s="1">
-        <v>19.30472727272727</v>
+        <v>-11.928761303944141</v>
       </c>
       <c r="J8" s="1">
-        <v>20.480866985083161</v>
+        <v>-14.380161144729369</v>
       </c>
       <c r="K8" s="1">
-        <v>26.2551782386615</v>
+        <v>-16.18661133825594</v>
       </c>
       <c r="L8" s="1">
-        <v>17.263368862166342</v>
+        <v>-4.4066985645933077</v>
       </c>
       <c r="M8" s="1">
-        <v>38.76196055457919</v>
+        <v>15.430728241563051</v>
       </c>
       <c r="N8" s="1">
-        <v>15.909471350426291</v>
+        <v>8.7287746672785751</v>
       </c>
       <c r="O8" s="1">
-        <v>33.843367531155202</v>
+        <v>13.60895328629158</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1614,25 +2286,25 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1">
-        <v>-43.861038095838033</v>
+        <v>-9.1731870337842469</v>
       </c>
       <c r="X8" s="1">
-        <v>-65.19463210436632</v>
+        <v>-24.297741101942151</v>
       </c>
       <c r="Y8" s="1">
-        <v>-72.992809714099735</v>
+        <v>-32.270343427508038</v>
       </c>
       <c r="Z8" s="1">
-        <v>-85.505530973451329</v>
+        <v>-70.958751393534001</v>
       </c>
       <c r="AA8" s="1">
-        <v>-55.943464120760488</v>
+        <v>-16.601303420035769</v>
       </c>
       <c r="AB8" s="1">
-        <v>-36.21884180876517</v>
+        <v>3.2944277108433822</v>
       </c>
       <c r="AC8" s="1">
-        <v>-31.622762778743791</v>
+        <v>-2.4207421971000298</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
@@ -1642,506 +2314,758 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1">
-        <v>-10.61842318150944</v>
+        <v>10.50084012887114</v>
       </c>
       <c r="AL8" s="1">
-        <v>-14.29974879815207</v>
+        <v>8.875739644970416</v>
       </c>
       <c r="AM8" s="1">
-        <v>-34.437910923222468</v>
+        <v>-4.1974155379106346</v>
       </c>
       <c r="AN8" s="1">
-        <v>-61.131130716517781</v>
+        <v>-31.25060544415382</v>
       </c>
       <c r="AO8" s="1">
-        <v>-41.195657068478738</v>
+        <v>10.576305994095749</v>
       </c>
       <c r="AP8" s="1">
-        <v>-33.142343556903711</v>
+        <v>19.935281947907281</v>
       </c>
       <c r="AQ8" s="1">
-        <v>-30.675307188972671</v>
+        <v>21.68614357262102</v>
       </c>
       <c r="AR8" s="1">
-        <v>-52.150673388870793</v>
+        <v>-30.018959533474501</v>
       </c>
       <c r="AS8" s="1">
-        <v>-54.985987409406022</v>
+        <v>-38.314348192112668</v>
       </c>
       <c r="AT8" s="1">
-        <v>-54.373398572273068</v>
+        <v>-47.817707791982833</v>
       </c>
       <c r="AU8" s="1">
-        <v>-64.375802718921676</v>
+        <v>-88.282778864970638</v>
       </c>
       <c r="AV8" s="1">
-        <v>-60.8115837245617</v>
+        <v>-92.573908962928186</v>
       </c>
       <c r="AW8" s="1">
-        <v>-56.454200124915531</v>
+        <v>-95.032991202346025</v>
       </c>
       <c r="AX8" s="1">
-        <v>-55.085894951047962</v>
+        <v>-102.8591352859135</v>
+      </c>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+      <c r="BJ8" s="1"/>
+      <c r="BK8" s="1"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1"/>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
+      <c r="BV8" s="1"/>
+      <c r="BW8" s="1"/>
+      <c r="BX8" s="1"/>
+      <c r="BY8" s="1"/>
+      <c r="BZ8" s="1"/>
+      <c r="CA8" s="1"/>
+      <c r="CB8" s="1"/>
+      <c r="CC8" s="1"/>
+      <c r="CD8" s="1"/>
+      <c r="CE8" s="1"/>
+      <c r="CF8" s="1"/>
+      <c r="CG8" s="1"/>
+      <c r="CH8" s="1"/>
+      <c r="CI8" s="1"/>
+      <c r="CJ8" s="1"/>
+      <c r="CK8" s="1"/>
+      <c r="CL8" s="1"/>
+      <c r="CM8" s="1"/>
+      <c r="CN8" s="1"/>
+      <c r="CO8" s="1">
+        <v>-78.55280312907432</v>
+      </c>
+      <c r="CP8" s="1">
+        <v>-85.48012363874561</v>
+      </c>
+      <c r="CQ8" s="1">
+        <v>-91.669009794273407</v>
+      </c>
+      <c r="CR8" s="1">
+        <v>-124.5044845532056</v>
+      </c>
+      <c r="CS8" s="1">
+        <v>-116.96144547652371</v>
+      </c>
+      <c r="CT8" s="1">
+        <v>-111.135788585887</v>
+      </c>
+      <c r="CU8" s="1">
+        <v>-104.7497637206849</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1">
-        <v>-8.8237720216233484</v>
+        <v>-5.5063216353538964</v>
       </c>
       <c r="C9" s="1">
-        <v>-33.954551581595979</v>
+        <v>-14.32169845268082</v>
       </c>
       <c r="D9" s="1">
-        <v>-33.905058714067131</v>
+        <v>-10.7779605815398</v>
       </c>
       <c r="E9" s="1">
-        <v>-71.370411126426092</v>
+        <v>-70.879763511342446</v>
       </c>
       <c r="F9" s="1">
-        <v>-55.973171455493294</v>
+        <v>-48.889486662183373</v>
       </c>
       <c r="G9" s="1">
-        <v>-19.883515426298668</v>
+        <v>11.25183377215741</v>
       </c>
       <c r="H9" s="1">
-        <v>15.71876365838882</v>
+        <v>39.759816067322937</v>
       </c>
       <c r="I9" s="1">
-        <v>15.748926098009999</v>
+        <v>18.376312677666661</v>
       </c>
       <c r="J9" s="1">
-        <v>-4.8034867949831517</v>
+        <v>0.55165739172514816</v>
       </c>
       <c r="K9" s="1">
-        <v>-7.4675521961169027</v>
+        <v>-5.4969204927211637</v>
       </c>
       <c r="L9" s="1">
-        <v>-39.951439334349217</v>
+        <v>-9.5136265355097738</v>
       </c>
       <c r="M9" s="1">
-        <v>-38.60861400555293</v>
+        <v>-4.3905850782911493</v>
       </c>
       <c r="N9" s="1">
-        <v>-48.088920165802172</v>
+        <v>-28.701815710263119</v>
       </c>
       <c r="O9" s="1">
-        <v>-40.823168479815287</v>
+        <v>-24.72057494828859</v>
       </c>
       <c r="P9" s="1">
-        <v>-19.8701953937063</v>
+        <v>-33.388141721796607</v>
       </c>
       <c r="Q9" s="1">
-        <v>-50.833143198132589</v>
+        <v>-60.431991672449669</v>
       </c>
       <c r="R9" s="1">
-        <v>-60.436844303579761</v>
+        <v>-71.008707713647226</v>
       </c>
       <c r="S9" s="1">
-        <v>-65.61973053329065</v>
+        <v>-84.257362496971282</v>
       </c>
       <c r="T9" s="1">
-        <v>-28.205427246759591</v>
+        <v>-58.651661075641158</v>
       </c>
       <c r="U9" s="1">
-        <v>28.806438837985329</v>
+        <v>-2.0106865202967898</v>
       </c>
       <c r="V9" s="1">
-        <v>54.449692990322333</v>
+        <v>8.1898477506272247</v>
       </c>
       <c r="W9" s="1">
-        <v>-14.619468222114889</v>
+        <v>-9.8208780036204626</v>
       </c>
       <c r="X9" s="1">
-        <v>-38.479397244912839</v>
+        <v>-26.827771865022228</v>
       </c>
       <c r="Y9" s="1">
-        <v>-51.896422811206207</v>
+        <v>-43.056735538109102</v>
       </c>
       <c r="Z9" s="1">
-        <v>-83.892490303735883</v>
+        <v>-94.213209038624029</v>
       </c>
       <c r="AA9" s="1">
-        <v>-55.559436595955589</v>
+        <v>-57.421398976358759</v>
       </c>
       <c r="AB9" s="1">
-        <v>-51.353632563756733</v>
+        <v>-56.679024390243903</v>
       </c>
       <c r="AC9" s="1">
-        <v>-27.0930317696657</v>
+        <v>-39.261537022530383</v>
       </c>
       <c r="AD9" s="1">
-        <v>-26.84801612809682</v>
+        <v>-26.22780375482067</v>
       </c>
       <c r="AE9" s="1">
-        <v>-30.241968511896051</v>
+        <v>-31.645549881096251</v>
       </c>
       <c r="AF9" s="1">
-        <v>-28.599312895249358</v>
+        <v>-31.84137077397277</v>
       </c>
       <c r="AG9" s="1">
-        <v>-41.134379799947553</v>
+        <v>-55.819327000034797</v>
       </c>
       <c r="AH9" s="1">
-        <v>-24.44997285865896</v>
+        <v>-41.046048268188272</v>
       </c>
       <c r="AI9" s="1">
-        <v>-21.76466724906351</v>
+        <v>-20.400815217391301</v>
       </c>
       <c r="AJ9" s="1">
-        <v>-17.5527116941035</v>
+        <v>-12.07103833452542</v>
       </c>
       <c r="AK9" s="1">
-        <v>-3.879233379670302</v>
+        <v>13.37542644737513</v>
       </c>
       <c r="AL9" s="1">
-        <v>-2.0834786652714792</v>
+        <v>19.11078589199473</v>
       </c>
       <c r="AM9" s="1">
-        <v>-7.6760105509889884</v>
+        <v>15.881740165682819</v>
       </c>
       <c r="AN9" s="1">
-        <v>-14.587608631921009</v>
+        <v>39.367451791552682</v>
       </c>
       <c r="AO9" s="1">
-        <v>-11.253442419990041</v>
+        <v>18.172292934882851</v>
       </c>
       <c r="AP9" s="1">
-        <v>-22.71974694598693</v>
+        <v>8.7626140725926955</v>
       </c>
       <c r="AQ9" s="1">
-        <v>-28.765422933040131</v>
+        <v>-2.0727210256533151</v>
       </c>
       <c r="AR9" s="1">
-        <v>-63.257390923323527</v>
+        <v>2.1511734703249532</v>
       </c>
       <c r="AS9" s="1">
-        <v>-66.294296124595277</v>
+        <v>1.972421498829606</v>
       </c>
       <c r="AT9" s="1">
-        <v>-65.431353942933256</v>
+        <v>1.34696942545803</v>
       </c>
       <c r="AU9" s="1">
-        <v>-73.268434691387796</v>
+        <v>27.693239967681119</v>
       </c>
       <c r="AV9" s="1">
-        <v>-69.131914693853417</v>
+        <v>24.233550947260611</v>
       </c>
       <c r="AW9" s="1">
-        <v>-68.1337207833528</v>
+        <v>27.275762688035989</v>
       </c>
       <c r="AX9" s="1">
-        <v>-64.975339176900277</v>
+        <v>26.620148729733181</v>
+      </c>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
+      <c r="BJ9" s="1"/>
+      <c r="BK9" s="1"/>
+      <c r="BL9" s="1"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+      <c r="BQ9" s="1"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+      <c r="BT9" s="1"/>
+      <c r="BU9" s="1"/>
+      <c r="BV9" s="1"/>
+      <c r="BW9" s="1"/>
+      <c r="BX9" s="1"/>
+      <c r="BY9" s="1"/>
+      <c r="BZ9" s="1"/>
+      <c r="CA9" s="1"/>
+      <c r="CB9" s="1"/>
+      <c r="CC9" s="1"/>
+      <c r="CD9" s="1"/>
+      <c r="CE9" s="1"/>
+      <c r="CF9" s="1"/>
+      <c r="CG9" s="1"/>
+      <c r="CH9" s="1"/>
+      <c r="CI9" s="1"/>
+      <c r="CJ9" s="1"/>
+      <c r="CK9" s="1"/>
+      <c r="CL9" s="1"/>
+      <c r="CM9" s="1"/>
+      <c r="CN9" s="1"/>
+      <c r="CO9" s="1">
+        <v>32.968900645225077</v>
+      </c>
+      <c r="CP9" s="1">
+        <v>26.58367492052869</v>
+      </c>
+      <c r="CQ9" s="1">
+        <v>23.716614637530341</v>
+      </c>
+      <c r="CR9" s="1">
+        <v>68.93535819352789</v>
+      </c>
+      <c r="CS9" s="1">
+        <v>49.574264125408817</v>
+      </c>
+      <c r="CT9" s="1">
+        <v>39.642011055540927</v>
+      </c>
+      <c r="CU9" s="1">
+        <v>77.54148340663734</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="B10" s="1">
-        <v>-38.035422014340938</v>
+        <v>9.6785109983079423</v>
       </c>
       <c r="C10" s="1">
-        <v>-48.052965454092742</v>
+        <v>-3.6941150875666282</v>
       </c>
       <c r="D10" s="1">
-        <v>-52.09948100774001</v>
+        <v>-3.181214471657015</v>
       </c>
       <c r="E10" s="1">
-        <v>-62.853573124551083</v>
+        <v>-10.52156921689463</v>
       </c>
       <c r="F10" s="1">
-        <v>-55.825574282731779</v>
+        <v>-17.13348320068048</v>
       </c>
       <c r="G10" s="1">
-        <v>-49.236120501642063</v>
+        <v>-14.16220913681245</v>
       </c>
       <c r="H10" s="1">
-        <v>-35.19922298763845</v>
+        <v>0.37340069188951491</v>
       </c>
       <c r="I10" s="1">
-        <v>-14.32719069419854</v>
+        <v>-20.97456783899597</v>
       </c>
       <c r="J10" s="1">
-        <v>-16.58659489485375</v>
+        <v>-21.186831620884892</v>
       </c>
       <c r="K10" s="1">
-        <v>-17.09081959143489</v>
+        <v>-44.960198124889438</v>
       </c>
       <c r="L10" s="1">
-        <v>-64.707700550186487</v>
+        <v>-88.802818200261896</v>
       </c>
       <c r="M10" s="1">
-        <v>-60.804794041051792</v>
+        <v>-71.098713776538048</v>
       </c>
       <c r="N10" s="1">
-        <v>-54.871685494715557</v>
+        <v>-62.785846420277871</v>
       </c>
       <c r="O10" s="1">
-        <v>-48.193562273145062</v>
+        <v>-47.536131942648623</v>
       </c>
       <c r="P10" s="1">
-        <v>23.75151587162382</v>
+        <v>-4.565940155153311</v>
       </c>
       <c r="Q10" s="1">
-        <v>9.4766340983109831</v>
+        <v>-17.140824473340981</v>
       </c>
       <c r="R10" s="1">
-        <v>7.9115883395672766</v>
+        <v>-22.736559540675572</v>
       </c>
       <c r="S10" s="1">
-        <v>21.609150758355501</v>
+        <v>-40.986142654948821</v>
       </c>
       <c r="T10" s="1">
-        <v>-4.5468214350153344</v>
+        <v>-39.167882422867031</v>
       </c>
       <c r="U10" s="1">
-        <v>-16.686822622035439</v>
+        <v>-37.003938701883293</v>
       </c>
       <c r="V10" s="1">
-        <v>80.542630856348211</v>
+        <v>34.756299342882798</v>
       </c>
       <c r="W10" s="1">
-        <v>47.368378931193767</v>
+        <v>29.0050379900553</v>
       </c>
       <c r="X10" s="1">
-        <v>64.544158705597425</v>
+        <v>34.904841993449587</v>
       </c>
       <c r="Y10" s="1">
-        <v>95.117632777039233</v>
+        <v>45.40821033210333</v>
       </c>
       <c r="Z10" s="1">
-        <v>40.170359989489363</v>
+        <v>-29.05738356382134</v>
       </c>
       <c r="AA10" s="1">
-        <v>-26.010406862820719</v>
+        <v>-45.256180478507019</v>
       </c>
       <c r="AB10" s="1">
-        <v>-18.528686364440691</v>
+        <v>-37.042948774792357</v>
       </c>
       <c r="AC10" s="1">
-        <v>-22.474101575813751</v>
+        <v>-42.349270887273619</v>
       </c>
       <c r="AD10" s="1">
-        <v>-4.1938900946497233</v>
+        <v>12.38306828811975</v>
       </c>
       <c r="AE10" s="1">
-        <v>-6.253226424613116</v>
+        <v>18.83758289739259</v>
       </c>
       <c r="AF10" s="1">
-        <v>-8.7798691968234941</v>
+        <v>25.087180675433029</v>
       </c>
       <c r="AG10" s="1">
-        <v>-20.890454836643169</v>
+        <v>33.653541644674327</v>
       </c>
       <c r="AH10" s="1">
-        <v>-27.05652202706796</v>
+        <v>1.6730975000810651</v>
       </c>
       <c r="AI10" s="1">
-        <v>-26.53361175531451</v>
+        <v>-2.5160077951002129</v>
       </c>
       <c r="AJ10" s="1">
-        <v>-19.680661406318439</v>
+        <v>2.5951557093425741</v>
       </c>
       <c r="AK10" s="1">
-        <v>-12.618584815996281</v>
+        <v>-25.389418655307601</v>
       </c>
       <c r="AL10" s="1">
-        <v>-17.665737009743331</v>
+        <v>-32.207607536437962</v>
       </c>
       <c r="AM10" s="1">
-        <v>-17.12548576401689</v>
+        <v>-24.679720798072768</v>
       </c>
       <c r="AN10" s="1">
-        <v>-22.047848801651249</v>
+        <v>-50.166464599811391</v>
       </c>
       <c r="AO10" s="1">
-        <v>-21.400614570758751</v>
+        <v>-45.859899284944042</v>
       </c>
       <c r="AP10" s="1">
-        <v>-11.393213805276099</v>
+        <v>-38.998421265190728</v>
       </c>
       <c r="AQ10" s="1">
-        <v>-4.6930851879876752</v>
+        <v>-31.742384066937721</v>
       </c>
       <c r="AR10" s="1">
-        <v>-8.5491494108025439</v>
+        <v>4.8904037747556552</v>
       </c>
       <c r="AS10" s="1">
-        <v>-11.70061211779559</v>
+        <v>4.0605591713690004</v>
       </c>
       <c r="AT10" s="1">
-        <v>-11.682574180012249</v>
+        <v>2.249150022760892</v>
       </c>
       <c r="AU10" s="1">
-        <v>-33.205872906648906</v>
+        <v>-6.7994505494505377</v>
       </c>
       <c r="AV10" s="1">
-        <v>-35.495461513158908</v>
+        <v>-17.63507511682694</v>
       </c>
       <c r="AW10" s="1">
-        <v>-32.002813162946339</v>
+        <v>-27.546296296296291</v>
       </c>
       <c r="AX10" s="1">
-        <v>-20.94013679598859</v>
+        <v>-30.97830958142869</v>
+      </c>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+      <c r="BJ10" s="1"/>
+      <c r="BK10" s="1"/>
+      <c r="BL10" s="1"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+      <c r="BQ10" s="1"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+      <c r="BT10" s="1"/>
+      <c r="BU10" s="1"/>
+      <c r="BV10" s="1"/>
+      <c r="BW10" s="1"/>
+      <c r="BX10" s="1"/>
+      <c r="BY10" s="1"/>
+      <c r="BZ10" s="1"/>
+      <c r="CA10" s="1"/>
+      <c r="CB10" s="1"/>
+      <c r="CC10" s="1"/>
+      <c r="CD10" s="1"/>
+      <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
+      <c r="CG10" s="1"/>
+      <c r="CH10" s="1"/>
+      <c r="CI10" s="1"/>
+      <c r="CJ10" s="1"/>
+      <c r="CK10" s="1"/>
+      <c r="CL10" s="1"/>
+      <c r="CM10" s="1"/>
+      <c r="CN10" s="1"/>
+      <c r="CO10" s="1">
+        <v>-8.2982238928278793</v>
+      </c>
+      <c r="CP10" s="1">
+        <v>-5.899873983274138</v>
+      </c>
+      <c r="CQ10" s="1">
+        <v>-2.2747575753209621</v>
+      </c>
+      <c r="CR10" s="1">
+        <v>6.0980936632242324</v>
+      </c>
+      <c r="CS10" s="1">
+        <v>0.11916175866319501</v>
+      </c>
+      <c r="CT10" s="1">
+        <v>-3.6067424000785069</v>
+      </c>
+      <c r="CU10" s="1">
+        <v>18.626780803828051</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B11" s="1">
-        <v>-1.7627260302275489</v>
+        <v>-5.1860000000000017</v>
       </c>
       <c r="C11" s="1">
-        <v>-2.4050952438997562</v>
+        <v>-4.4379</v>
       </c>
       <c r="D11" s="1">
-        <v>-2.3790531417831491</v>
+        <v>-3.6075999999999988</v>
       </c>
       <c r="E11" s="1">
-        <v>-2.3347377993298051</v>
+        <v>-4.9370833333333337</v>
       </c>
       <c r="F11" s="1">
-        <v>-2.7290858020702569</v>
+        <v>-4.712416666666666</v>
       </c>
       <c r="G11" s="1">
-        <v>-0.27832451270945091</v>
+        <v>-3.9941249999999981</v>
       </c>
       <c r="H11" s="1">
-        <v>1.307452290332656</v>
+        <v>-3.708333333333333</v>
       </c>
       <c r="I11" s="1">
-        <v>2.3787575563325571</v>
+        <v>0.80056250000000029</v>
       </c>
       <c r="J11" s="1">
-        <v>1.398779797979798</v>
+        <v>-0.17551249999999971</v>
       </c>
       <c r="K11" s="1">
-        <v>1.594316317016317</v>
+        <v>-0.1386750000000001</v>
       </c>
       <c r="L11" s="1">
-        <v>1.6616432109557111</v>
+        <v>2.484458333333333</v>
       </c>
       <c r="M11" s="1">
-        <v>2.7936463918026422</v>
+        <v>5.3694166666666661</v>
       </c>
       <c r="N11" s="1">
-        <v>0.27914464840714848</v>
+        <v>3.415541666666666</v>
       </c>
       <c r="O11" s="1">
-        <v>1.1649409805880391</v>
+        <v>4.2302916666666652</v>
       </c>
       <c r="P11" s="1">
-        <v>-3.5414489623865122</v>
+        <v>-5.1148999999999996</v>
       </c>
       <c r="Q11" s="1">
-        <v>-3.607477777777778</v>
+        <v>-4.2444999999999986</v>
       </c>
       <c r="R11" s="1">
-        <v>-3.4348055555555548</v>
+        <v>-4.0769500000000001</v>
       </c>
       <c r="S11" s="1">
-        <v>-2.523545673076923</v>
+        <v>-3.5855000000000001</v>
       </c>
       <c r="T11" s="1">
-        <v>-3.2737500000000002</v>
+        <v>-4.7855833333333333</v>
       </c>
       <c r="U11" s="1">
-        <v>-1.965257211538461</v>
+        <v>-5.3800833333333333</v>
       </c>
       <c r="V11" s="1">
-        <v>0.73828867057757819</v>
+        <v>-6.1934999999999976</v>
       </c>
       <c r="W11" s="1">
-        <v>-0.5190749007936506</v>
+        <v>-1.934287500000001</v>
       </c>
       <c r="X11" s="1">
-        <v>-2.8137428075396822</v>
+        <v>-3.0287999999999999</v>
       </c>
       <c r="Y11" s="1">
-        <v>-2.7254437003968262</v>
+        <v>-2.2165625000000002</v>
       </c>
       <c r="Z11" s="1">
-        <v>-5.0779242559523814</v>
+        <v>-5.4389583333333338</v>
       </c>
       <c r="AA11" s="1">
-        <v>-6.7655919642857141</v>
+        <v>-6.3373333333333326</v>
       </c>
       <c r="AB11" s="1">
-        <v>-6.8704421721187341</v>
+        <v>-6.8069583333333341</v>
       </c>
       <c r="AC11" s="1">
-        <v>-7.2199184383131527</v>
+        <v>-8.3651666666666671</v>
       </c>
       <c r="AD11" s="1">
-        <v>-8.1013883928571424</v>
+        <v>-4.6690500000000004</v>
       </c>
       <c r="AE11" s="1">
-        <v>-7.4546634424603164</v>
+        <v>-4.8903999999999996</v>
       </c>
       <c r="AF11" s="1">
-        <v>-6.3286515376984136</v>
+        <v>-4.24695</v>
       </c>
       <c r="AG11" s="1">
-        <v>-6.4207127976190472</v>
+        <v>-6.8088333333333333</v>
       </c>
       <c r="AH11" s="1">
-        <v>-8.2354794195804182</v>
+        <v>-9.3040833333333328</v>
       </c>
       <c r="AI11" s="1">
-        <v>-9.1135043859649123</v>
+        <v>-8.1286666666666676</v>
       </c>
       <c r="AJ11" s="1">
-        <v>-9.9600293390287771</v>
+        <v>-7.7480416666666656</v>
       </c>
       <c r="AK11" s="1">
-        <v>-4.5892503359385719</v>
+        <v>3.125883333333332</v>
       </c>
       <c r="AL11" s="1">
-        <v>-4.8251208624708619</v>
+        <v>2.333966666666667</v>
       </c>
       <c r="AM11" s="1">
-        <v>-4.8356510078157138</v>
+        <v>1.8866333333333329</v>
       </c>
       <c r="AN11" s="1">
-        <v>-5.2643591790154289</v>
+        <v>2.5846666666666671</v>
       </c>
       <c r="AO11" s="1">
-        <v>-5.2562782235125987</v>
+        <v>1.5189166666666669</v>
       </c>
       <c r="AP11" s="1">
-        <v>-7.4399353632478622</v>
+        <v>0.93125000000000058</v>
       </c>
       <c r="AQ11" s="1">
-        <v>-8.9401810099622594</v>
+        <v>-0.50274999999999959</v>
       </c>
       <c r="AR11" s="1">
-        <v>-5.9376441746189119</v>
+        <v>1.252242307692307</v>
       </c>
       <c r="AS11" s="1">
-        <v>-4.249854099856166</v>
+        <v>0.44091463414634252</v>
       </c>
       <c r="AT11" s="1">
-        <v>-4.9622967281341426</v>
+        <v>9.6577586206896354E-2</v>
       </c>
       <c r="AU11" s="1">
-        <v>-4.6589588971033979</v>
+        <v>3.49125</v>
       </c>
       <c r="AV11" s="1">
-        <v>-6.5228971797569946</v>
+        <v>4.7644999999999991</v>
       </c>
       <c r="AW11" s="1">
-        <v>-7.525353939503387</v>
+        <v>6.3294999999999986</v>
       </c>
       <c r="AX11" s="1">
-        <v>-8.6235365299191216</v>
+        <v>6.81</v>
+      </c>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
+      <c r="BP11" s="1"/>
+      <c r="BQ11" s="1"/>
+      <c r="BR11" s="1"/>
+      <c r="BS11" s="1"/>
+      <c r="BT11" s="1"/>
+      <c r="BU11" s="1"/>
+      <c r="BV11" s="1"/>
+      <c r="BW11" s="1"/>
+      <c r="BX11" s="1"/>
+      <c r="BY11" s="1"/>
+      <c r="BZ11" s="1"/>
+      <c r="CA11" s="1"/>
+      <c r="CB11" s="1"/>
+      <c r="CC11" s="1"/>
+      <c r="CD11" s="1"/>
+      <c r="CE11" s="1"/>
+      <c r="CF11" s="1"/>
+      <c r="CG11" s="1"/>
+      <c r="CH11" s="1"/>
+      <c r="CI11" s="1"/>
+      <c r="CJ11" s="1"/>
+      <c r="CK11" s="1"/>
+      <c r="CL11" s="1"/>
+      <c r="CM11" s="1"/>
+      <c r="CN11" s="1"/>
+      <c r="CO11" s="1">
+        <v>-2.8838124999999999</v>
+      </c>
+      <c r="CP11" s="1">
+        <v>-3.9068125</v>
+      </c>
+      <c r="CQ11" s="1">
+        <v>-3.3939374999999998</v>
+      </c>
+      <c r="CR11" s="1">
+        <v>-4.4002499999999998</v>
+      </c>
+      <c r="CS11" s="1">
+        <v>0.18624999999999969</v>
+      </c>
+      <c r="CT11" s="1">
+        <v>-0.99225000000000008</v>
+      </c>
+      <c r="CU11" s="1">
+        <v>-0.98949999999999982</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AX11">
+  <conditionalFormatting sqref="A1:CU11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Add a new way to work with the timezone & modify graphs & automatisation
</commit_message>
<xml_diff>
--- a/plots/alerts_ech.xlsx
+++ b/plots/alerts_ech.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0E55D6AD87205348F31B3F11595ED87656CD6549" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33BEB7A4-DDD5-9F41-8A6C-3B73D9BF3891}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_5E1534BF87D0531AD3F83C11595ED87656CDFA1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{931237D7-E392-4A4A-A64C-D7A29A9A37BD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35400" yWindow="3820" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>A1-12h</t>
   </si>
@@ -199,7 +199,7 @@
     <t>A9-3h</t>
   </si>
   <si>
-    <t>Jeudi1 Septembre 6h - 12h</t>
+    <t>Jeudi1 Septembre 17h - 23h</t>
   </si>
   <si>
     <t>A9+3h</t>
@@ -314,6 +314,48 @@
   </si>
   <si>
     <t>A14+12h</t>
+  </si>
+  <si>
+    <t>A15-12h</t>
+  </si>
+  <si>
+    <t>A15-6h</t>
+  </si>
+  <si>
+    <t>A15-3h</t>
+  </si>
+  <si>
+    <t>Dimanche4 Decembre 12h - 18h</t>
+  </si>
+  <si>
+    <t>A15+3h</t>
+  </si>
+  <si>
+    <t>A15+6h</t>
+  </si>
+  <si>
+    <t>A15+12h</t>
+  </si>
+  <si>
+    <t>A16-12h</t>
+  </si>
+  <si>
+    <t>A16-6h</t>
+  </si>
+  <si>
+    <t>A16-3h</t>
+  </si>
+  <si>
+    <t>Lundi19 Decembre 16h - 22h</t>
+  </si>
+  <si>
+    <t>A16+3h</t>
+  </si>
+  <si>
+    <t>A16+6h</t>
+  </si>
+  <si>
+    <t>A16+12h</t>
   </si>
   <si>
     <t>ECHL01</t>
@@ -707,15 +749,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU11"/>
+  <dimension ref="A1:DI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="A1:CU11"/>
+      <selection activeCell="CW18" sqref="CW18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1011,10 +1057,52 @@
       <c r="CU1" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="CV1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1">
         <v>-8.5820673740887656</v>
@@ -1198,10 +1286,24 @@
       <c r="CU2" s="1">
         <v>82.36492590385761</v>
       </c>
+      <c r="CV2" s="1"/>
+      <c r="CW2" s="1"/>
+      <c r="CX2" s="1"/>
+      <c r="CY2" s="1"/>
+      <c r="CZ2" s="1"/>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1"/>
+      <c r="DC2" s="1"/>
+      <c r="DD2" s="1"/>
+      <c r="DE2" s="1"/>
+      <c r="DF2" s="1"/>
+      <c r="DG2" s="1"/>
+      <c r="DH2" s="1"/>
+      <c r="DI2" s="1"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1">
         <v>-17.789749933523709</v>
@@ -1413,10 +1515,24 @@
       <c r="CU3" s="1">
         <v>-45.200777520791299</v>
       </c>
+      <c r="CV3" s="1"/>
+      <c r="CW3" s="1"/>
+      <c r="CX3" s="1"/>
+      <c r="CY3" s="1"/>
+      <c r="CZ3" s="1"/>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1"/>
+      <c r="DC3" s="1"/>
+      <c r="DD3" s="1"/>
+      <c r="DE3" s="1"/>
+      <c r="DF3" s="1"/>
+      <c r="DG3" s="1"/>
+      <c r="DH3" s="1"/>
+      <c r="DI3" s="1"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1">
         <v>-9.2726242206687992</v>
@@ -1614,10 +1730,24 @@
       <c r="CU4" s="1">
         <v>32.197631527858682</v>
       </c>
+      <c r="CV4" s="1"/>
+      <c r="CW4" s="1"/>
+      <c r="CX4" s="1"/>
+      <c r="CY4" s="1"/>
+      <c r="CZ4" s="1"/>
+      <c r="DA4" s="1"/>
+      <c r="DB4" s="1"/>
+      <c r="DC4" s="1"/>
+      <c r="DD4" s="1"/>
+      <c r="DE4" s="1"/>
+      <c r="DF4" s="1"/>
+      <c r="DG4" s="1"/>
+      <c r="DH4" s="1"/>
+      <c r="DI4" s="1"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B5" s="1">
         <v>-55.646703573225963</v>
@@ -1829,10 +1959,24 @@
       <c r="CU5" s="1">
         <v>17.626315850424429</v>
       </c>
+      <c r="CV5" s="1"/>
+      <c r="CW5" s="1"/>
+      <c r="CX5" s="1"/>
+      <c r="CY5" s="1"/>
+      <c r="CZ5" s="1"/>
+      <c r="DA5" s="1"/>
+      <c r="DB5" s="1"/>
+      <c r="DC5" s="1"/>
+      <c r="DD5" s="1"/>
+      <c r="DE5" s="1"/>
+      <c r="DF5" s="1"/>
+      <c r="DG5" s="1"/>
+      <c r="DH5" s="1"/>
+      <c r="DI5" s="1"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1">
         <v>-15.26533477816273</v>
@@ -2016,10 +2160,24 @@
       <c r="CU6" s="1">
         <v>-86.744409384003291</v>
       </c>
+      <c r="CV6" s="1"/>
+      <c r="CW6" s="1"/>
+      <c r="CX6" s="1"/>
+      <c r="CY6" s="1"/>
+      <c r="CZ6" s="1"/>
+      <c r="DA6" s="1"/>
+      <c r="DB6" s="1"/>
+      <c r="DC6" s="1"/>
+      <c r="DD6" s="1"/>
+      <c r="DE6" s="1"/>
+      <c r="DF6" s="1"/>
+      <c r="DG6" s="1"/>
+      <c r="DH6" s="1"/>
+      <c r="DI6" s="1"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1">
         <v>10.467373477563379</v>
@@ -2231,10 +2389,24 @@
       <c r="CU7" s="1">
         <v>-64.498176933410093</v>
       </c>
+      <c r="CV7" s="1"/>
+      <c r="CW7" s="1"/>
+      <c r="CX7" s="1"/>
+      <c r="CY7" s="1"/>
+      <c r="CZ7" s="1"/>
+      <c r="DA7" s="1"/>
+      <c r="DB7" s="1"/>
+      <c r="DC7" s="1"/>
+      <c r="DD7" s="1"/>
+      <c r="DE7" s="1"/>
+      <c r="DF7" s="1"/>
+      <c r="DG7" s="1"/>
+      <c r="DH7" s="1"/>
+      <c r="DI7" s="1"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1">
         <v>-23.241633082179771</v>
@@ -2418,10 +2590,24 @@
       <c r="CU8" s="1">
         <v>-104.7497637206849</v>
       </c>
+      <c r="CV8" s="1"/>
+      <c r="CW8" s="1"/>
+      <c r="CX8" s="1"/>
+      <c r="CY8" s="1"/>
+      <c r="CZ8" s="1"/>
+      <c r="DA8" s="1"/>
+      <c r="DB8" s="1"/>
+      <c r="DC8" s="1"/>
+      <c r="DD8" s="1"/>
+      <c r="DE8" s="1"/>
+      <c r="DF8" s="1"/>
+      <c r="DG8" s="1"/>
+      <c r="DH8" s="1"/>
+      <c r="DI8" s="1"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1">
         <v>-5.5063216353538964</v>
@@ -2633,10 +2819,24 @@
       <c r="CU9" s="1">
         <v>77.54148340663734</v>
       </c>
+      <c r="CV9" s="1"/>
+      <c r="CW9" s="1"/>
+      <c r="CX9" s="1"/>
+      <c r="CY9" s="1"/>
+      <c r="CZ9" s="1"/>
+      <c r="DA9" s="1"/>
+      <c r="DB9" s="1"/>
+      <c r="DC9" s="1"/>
+      <c r="DD9" s="1"/>
+      <c r="DE9" s="1"/>
+      <c r="DF9" s="1"/>
+      <c r="DG9" s="1"/>
+      <c r="DH9" s="1"/>
+      <c r="DI9" s="1"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1">
         <v>9.6785109983079423</v>
@@ -2848,10 +3048,24 @@
       <c r="CU10" s="1">
         <v>18.626780803828051</v>
       </c>
+      <c r="CV10" s="1"/>
+      <c r="CW10" s="1"/>
+      <c r="CX10" s="1"/>
+      <c r="CY10" s="1"/>
+      <c r="CZ10" s="1"/>
+      <c r="DA10" s="1"/>
+      <c r="DB10" s="1"/>
+      <c r="DC10" s="1"/>
+      <c r="DD10" s="1"/>
+      <c r="DE10" s="1"/>
+      <c r="DF10" s="1"/>
+      <c r="DG10" s="1"/>
+      <c r="DH10" s="1"/>
+      <c r="DI10" s="1"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1">
         <v>-5.1860000000000017</v>
@@ -3063,9 +3277,23 @@
       <c r="CU11" s="1">
         <v>-0.98949999999999982</v>
       </c>
+      <c r="CV11" s="1"/>
+      <c r="CW11" s="1"/>
+      <c r="CX11" s="1"/>
+      <c r="CY11" s="1"/>
+      <c r="CZ11" s="1"/>
+      <c r="DA11" s="1"/>
+      <c r="DB11" s="1"/>
+      <c r="DC11" s="1"/>
+      <c r="DD11" s="1"/>
+      <c r="DE11" s="1"/>
+      <c r="DF11" s="1"/>
+      <c r="DG11" s="1"/>
+      <c r="DH11" s="1"/>
+      <c r="DI11" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:CU11">
+  <conditionalFormatting sqref="A1:DI11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Mise à jour des tableaux
</commit_message>
<xml_diff>
--- a/plots/alerts_ech.xlsx
+++ b/plots/alerts_ech.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_4E3D57AB870053469B592F11595ED87656CCE73F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D11D4334-DA92-314B-9012-951ACD0DA7DE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_667555A28730D766333B3711595ED87656CCB718" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C582A8B-5D83-EC46-BBD3-859DB5FBDF62}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34460" yWindow="2040" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,13 +519,15 @@
   <dimension ref="A1:DW15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:127" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -951,13 +953,6 @@
       <c r="O2" s="1">
         <v>3.5218873766281722</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
       <c r="W2" s="1">
         <v>19.614931321123318</v>
       </c>
@@ -979,13 +974,6 @@
       <c r="AC2" s="1">
         <v>-13.450852035704131</v>
       </c>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
       <c r="AK2" s="1">
         <v>-24.700312989859061</v>
       </c>
@@ -1348,13 +1336,6 @@
       <c r="AC3" s="1">
         <v>94.617074562425429</v>
       </c>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
       <c r="AK3" s="1">
         <v>-24.915197943619209</v>
       </c>
@@ -2441,13 +2422,6 @@
       <c r="O6" s="1">
         <v>-4.9465278993547166</v>
       </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
       <c r="W6" s="1">
         <v>19.066051461265491</v>
       </c>
@@ -2741,27 +2715,6 @@
       </c>
       <c r="DP6" s="1">
         <v>-20.980014434310441</v>
-      </c>
-      <c r="DQ6" s="1">
-        <v>-10.84523357211893</v>
-      </c>
-      <c r="DR6" s="1">
-        <v>-15.916403991420641</v>
-      </c>
-      <c r="DS6" s="1">
-        <v>19.191302625792581</v>
-      </c>
-      <c r="DT6" s="1">
-        <v>-81.745957874802329</v>
-      </c>
-      <c r="DU6" s="1">
-        <v>-3.258102483790482</v>
-      </c>
-      <c r="DV6" s="1">
-        <v>-8.3873508885151473</v>
-      </c>
-      <c r="DW6" s="1">
-        <v>7.133395575472008</v>
       </c>
     </row>
     <row r="7" spans="1:127" x14ac:dyDescent="0.2">
@@ -3193,13 +3146,6 @@
       <c r="O8" s="1">
         <v>13.480854629202019</v>
       </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
       <c r="W8" s="1">
         <v>9.0581765003724026</v>
       </c>
@@ -3221,13 +3167,6 @@
       <c r="AC8" s="1">
         <v>21.57315993606397</v>
       </c>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
       <c r="AK8" s="1">
         <v>4.5100071579421046</v>
       </c>
@@ -3931,13 +3870,6 @@
       <c r="O10" s="1">
         <v>45.499740018399912</v>
       </c>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
       <c r="W10" s="1">
         <v>-21.978871806758502</v>
       </c>
@@ -3959,13 +3891,6 @@
       <c r="AC10" s="1">
         <v>13.22655271642355</v>
       </c>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
       <c r="AK10" s="1">
         <v>25.978478718726599</v>
       </c>
@@ -5010,13 +4935,6 @@
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
       <c r="I13" s="1">
         <v>270.53787105366013</v>
       </c>
@@ -5038,13 +4956,6 @@
       <c r="O13" s="1">
         <v>-46.935101266756817</v>
       </c>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
       <c r="W13" s="1">
         <v>-26.171958836480879</v>
       </c>
@@ -5087,13 +4998,6 @@
       <c r="AJ13" s="1">
         <v>-16.336371774554699</v>
       </c>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
       <c r="AR13" s="1">
         <v>-19.20119293833643</v>
       </c>
@@ -6092,30 +5996,30 @@
         <v>507.96093074938858</v>
       </c>
       <c r="DQ15" s="1">
-        <v>3220.820136532689</v>
+        <v>3295.7820841172788</v>
       </c>
       <c r="DR15" s="1">
-        <v>4912.807330973008</v>
+        <v>5029.6733328161008</v>
       </c>
       <c r="DS15" s="1">
-        <v>4575.1531898772519</v>
+        <v>4433.4224448839614</v>
       </c>
       <c r="DT15" s="1">
-        <v>-1776.9883131363861</v>
+        <v>-1457.756570003947</v>
       </c>
       <c r="DU15" s="1">
-        <v>-2972.7864559628151</v>
+        <v>-2948.2025437006669</v>
       </c>
       <c r="DV15" s="1">
-        <v>-1893.9935293292649</v>
+        <v>-1840.4704859698161</v>
       </c>
       <c r="DW15" s="1">
-        <v>-1375.757675499186</v>
+        <v>-1423.898714682962</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:XFD14">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>